<commit_message>
Make Three Version fo film
</commit_message>
<xml_diff>
--- a/Descriptive Data/pdata/FilmCompare.xlsx
+++ b/Descriptive Data/pdata/FilmCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
   <si>
     <t>樂翻天新聞</t>
   </si>
@@ -187,6 +187,99 @@
   <si>
     <t>?人氣</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的美麗與哀愁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">以懸疑的情節，突破從校園到社會的重重禁忌，充分討論了青少年的蒙味感覺。  </t>
+  </si>
+  <si>
+    <t>影子軍團</t>
+  </si>
+  <si>
+    <t>坦克大決戰</t>
+  </si>
+  <si>
+    <t>二次世界大戰，德軍節節敗退之際，集中精銳的裝甲部隊與同盟國進行最後決戰。</t>
+  </si>
+  <si>
+    <t>轟炸超人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代表正義與邪惡的超人們，將以手中的炸彈做勝負對決。                      </t>
+  </si>
+  <si>
+    <t>荒山孤墳</t>
+  </si>
+  <si>
+    <t>科學新疆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">科學知識日新月異，吸引著求知慾望強盛的人鑽研其中。                      </t>
+  </si>
+  <si>
+    <t>天堂旅行團</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">由靈異人士帶領，經由特殊儀式，讓靈魂出竅前往天堂參觀。                  </t>
+  </si>
+  <si>
+    <t>９９衝鋒飛車賽</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">講求速度與靈動的機車比賽是少年追風少年的最愛！                          </t>
+  </si>
+  <si>
+    <t>蜜桃成熟時</t>
+  </si>
+  <si>
+    <t xml:space="preserve">且看女主角如何經過歷練而成熟……                                        </t>
+  </si>
+  <si>
+    <t>Ｋ－１９</t>
+  </si>
+  <si>
+    <t>movi-a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蘇聯潛艇發生核能外洩意外，要如何挽救呢？                                </t>
+  </si>
+  <si>
+    <t>遠離家園</t>
+  </si>
+  <si>
+    <t>小甜甜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小甜甜從小生長在孤兒院，她既美麗又大方，是一個人見人愛的女子。          </t>
+  </si>
+  <si>
+    <t>大家來守法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">各種生活中常遇到的法律問題。                                            </t>
+  </si>
+  <si>
+    <t>超級比一比　　　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">集合各種社會團體，在各項運動設施中拼一拼，看看誰奪得冠軍！              </t>
+  </si>
+  <si>
+    <t>龍舟大會</t>
+  </si>
+  <si>
+    <t>spe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龍舟中國節日的特有運動，講求團隊的默契。                                </t>
   </si>
 </sst>
 </file>
@@ -1152,9 +1245,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG15"/>
+  <dimension ref="A1:BG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -3301,6 +3396,2870 @@
         <v>45</v>
       </c>
     </row>
+    <row r="19" spans="1:59" s="11" customFormat="1">
+      <c r="A19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="11">
+        <v>11</v>
+      </c>
+      <c r="G19" s="11">
+        <v>884</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1</v>
+      </c>
+      <c r="I19" s="11">
+        <v>6</v>
+      </c>
+      <c r="J19" s="11">
+        <v>6</v>
+      </c>
+      <c r="K19" s="11">
+        <v>2</v>
+      </c>
+      <c r="L19" s="11">
+        <v>2</v>
+      </c>
+      <c r="M19" s="11">
+        <v>1</v>
+      </c>
+      <c r="N19" s="11">
+        <v>1995</v>
+      </c>
+      <c r="O19" s="11">
+        <v>4</v>
+      </c>
+      <c r="P19" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>2</v>
+      </c>
+      <c r="R19" s="11">
+        <v>0</v>
+      </c>
+      <c r="S19" s="11">
+        <v>0</v>
+      </c>
+      <c r="T19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U19" s="11">
+        <v>3</v>
+      </c>
+      <c r="V19" s="11">
+        <v>0</v>
+      </c>
+      <c r="W19" s="11">
+        <v>1</v>
+      </c>
+      <c r="X19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA19" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB19" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC19" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="11">
+        <v>900</v>
+      </c>
+      <c r="AI19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK19" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO19" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP19" s="11">
+        <v>30</v>
+      </c>
+      <c r="AQ19" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF19" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG19" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59" s="11" customFormat="1">
+      <c r="A20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="11">
+        <v>66</v>
+      </c>
+      <c r="G20" s="11">
+        <v>552</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="11">
+        <v>7</v>
+      </c>
+      <c r="J20" s="11">
+        <v>4</v>
+      </c>
+      <c r="K20" s="11">
+        <v>4</v>
+      </c>
+      <c r="L20" s="11">
+        <v>4</v>
+      </c>
+      <c r="M20" s="11">
+        <v>1</v>
+      </c>
+      <c r="N20" s="11">
+        <v>1997</v>
+      </c>
+      <c r="O20" s="11">
+        <v>0</v>
+      </c>
+      <c r="P20" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>2</v>
+      </c>
+      <c r="R20" s="11">
+        <v>0</v>
+      </c>
+      <c r="S20" s="11">
+        <v>0</v>
+      </c>
+      <c r="T20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U20" s="11">
+        <v>3</v>
+      </c>
+      <c r="V20" s="11">
+        <v>19</v>
+      </c>
+      <c r="W20" s="11">
+        <v>9</v>
+      </c>
+      <c r="X20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA20" s="11">
+        <v>6</v>
+      </c>
+      <c r="AB20" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>700</v>
+      </c>
+      <c r="AI20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK20" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO20" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP20" s="11">
+        <v>40</v>
+      </c>
+      <c r="AQ20" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF20" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG20" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59" s="11" customFormat="1">
+      <c r="A21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="11">
+        <v>42</v>
+      </c>
+      <c r="G21" s="11">
+        <v>244</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11">
+        <v>7</v>
+      </c>
+      <c r="J21" s="11">
+        <v>6</v>
+      </c>
+      <c r="K21" s="11">
+        <v>5</v>
+      </c>
+      <c r="L21" s="11">
+        <v>4</v>
+      </c>
+      <c r="M21" s="11">
+        <v>1</v>
+      </c>
+      <c r="N21" s="11">
+        <v>1976</v>
+      </c>
+      <c r="O21" s="11">
+        <v>0</v>
+      </c>
+      <c r="P21" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>2</v>
+      </c>
+      <c r="R21" s="11">
+        <v>0</v>
+      </c>
+      <c r="S21" s="11">
+        <v>0</v>
+      </c>
+      <c r="T21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U21" s="11">
+        <v>3</v>
+      </c>
+      <c r="V21" s="11">
+        <v>19</v>
+      </c>
+      <c r="W21" s="11">
+        <v>17</v>
+      </c>
+      <c r="X21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA21" s="11">
+        <v>7</v>
+      </c>
+      <c r="AB21" s="11">
+        <v>3</v>
+      </c>
+      <c r="AC21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="11">
+        <v>400</v>
+      </c>
+      <c r="AI21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK21" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO21" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP21" s="11">
+        <v>30</v>
+      </c>
+      <c r="AQ21" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG21" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:59" s="11" customFormat="1">
+      <c r="A22" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="11">
+        <v>31</v>
+      </c>
+      <c r="G22" s="11">
+        <v>109</v>
+      </c>
+      <c r="H22" s="11">
+        <v>2</v>
+      </c>
+      <c r="I22" s="11">
+        <v>11</v>
+      </c>
+      <c r="J22" s="11">
+        <v>4</v>
+      </c>
+      <c r="K22" s="11">
+        <v>3</v>
+      </c>
+      <c r="L22" s="11">
+        <v>5</v>
+      </c>
+      <c r="M22" s="11">
+        <v>1</v>
+      </c>
+      <c r="N22" s="11">
+        <v>1998</v>
+      </c>
+      <c r="O22" s="11">
+        <v>2</v>
+      </c>
+      <c r="P22" s="11">
+        <v>40</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>1</v>
+      </c>
+      <c r="R22" s="11">
+        <v>0</v>
+      </c>
+      <c r="S22" s="11">
+        <v>0</v>
+      </c>
+      <c r="T22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U22" s="11">
+        <v>3</v>
+      </c>
+      <c r="V22" s="11">
+        <v>6</v>
+      </c>
+      <c r="W22" s="11">
+        <v>19</v>
+      </c>
+      <c r="X22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA22" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="11">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="11">
+        <v>2300</v>
+      </c>
+      <c r="AI22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK22" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO22" s="11">
+        <v>38</v>
+      </c>
+      <c r="AP22" s="11">
+        <v>40</v>
+      </c>
+      <c r="AQ22" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF22" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG22" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59" s="11" customFormat="1">
+      <c r="A23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="11">
+        <v>33</v>
+      </c>
+      <c r="G23" s="11">
+        <v>328</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2</v>
+      </c>
+      <c r="I23" s="11">
+        <v>9</v>
+      </c>
+      <c r="J23" s="11">
+        <v>4</v>
+      </c>
+      <c r="K23" s="11">
+        <v>4</v>
+      </c>
+      <c r="L23" s="11">
+        <v>3</v>
+      </c>
+      <c r="M23" s="11">
+        <v>1</v>
+      </c>
+      <c r="N23" s="11">
+        <v>1998</v>
+      </c>
+      <c r="O23" s="11">
+        <v>0</v>
+      </c>
+      <c r="P23" s="11">
+        <v>40</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>1</v>
+      </c>
+      <c r="R23" s="11">
+        <v>0</v>
+      </c>
+      <c r="S23" s="11">
+        <v>0</v>
+      </c>
+      <c r="T23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U23" s="11">
+        <v>4</v>
+      </c>
+      <c r="V23" s="11">
+        <v>0</v>
+      </c>
+      <c r="W23" s="11">
+        <v>0</v>
+      </c>
+      <c r="X23" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="11">
+        <v>4000</v>
+      </c>
+      <c r="AI23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK23" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO23" s="11">
+        <v>38</v>
+      </c>
+      <c r="AP23" s="11">
+        <v>40</v>
+      </c>
+      <c r="AQ23" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF23" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG23" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59" s="11" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="11">
+        <v>29</v>
+      </c>
+      <c r="G24" s="11">
+        <v>245</v>
+      </c>
+      <c r="H24" s="11">
+        <v>3</v>
+      </c>
+      <c r="I24" s="11">
+        <v>13</v>
+      </c>
+      <c r="J24" s="11">
+        <v>7</v>
+      </c>
+      <c r="K24" s="11">
+        <v>3</v>
+      </c>
+      <c r="L24" s="11">
+        <v>1</v>
+      </c>
+      <c r="M24" s="11">
+        <v>1</v>
+      </c>
+      <c r="N24" s="11">
+        <v>1998</v>
+      </c>
+      <c r="O24" s="11">
+        <v>0</v>
+      </c>
+      <c r="P24" s="11">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>1</v>
+      </c>
+      <c r="R24" s="11">
+        <v>0</v>
+      </c>
+      <c r="S24" s="11">
+        <v>0</v>
+      </c>
+      <c r="T24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U24" s="11">
+        <v>2</v>
+      </c>
+      <c r="V24" s="11">
+        <v>0</v>
+      </c>
+      <c r="W24" s="11">
+        <v>1</v>
+      </c>
+      <c r="X24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA24" s="11">
+        <v>5</v>
+      </c>
+      <c r="AB24" s="11">
+        <v>5</v>
+      </c>
+      <c r="AC24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="11">
+        <v>4820</v>
+      </c>
+      <c r="AI24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK24" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO24" s="11">
+        <v>35</v>
+      </c>
+      <c r="AP24" s="11">
+        <v>20</v>
+      </c>
+      <c r="AQ24" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF24" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG24" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:59" s="11" customFormat="1">
+      <c r="A25" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="11">
+        <v>10</v>
+      </c>
+      <c r="G25" s="11">
+        <v>300</v>
+      </c>
+      <c r="H25" s="11">
+        <v>5</v>
+      </c>
+      <c r="I25" s="11">
+        <v>24</v>
+      </c>
+      <c r="J25" s="11">
+        <v>2</v>
+      </c>
+      <c r="K25" s="11">
+        <v>3</v>
+      </c>
+      <c r="L25" s="11">
+        <v>2</v>
+      </c>
+      <c r="M25" s="11">
+        <v>1</v>
+      </c>
+      <c r="N25" s="11">
+        <v>1999</v>
+      </c>
+      <c r="O25" s="11">
+        <v>4</v>
+      </c>
+      <c r="P25" s="11">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>2</v>
+      </c>
+      <c r="R25" s="11">
+        <v>0</v>
+      </c>
+      <c r="S25" s="11">
+        <v>0</v>
+      </c>
+      <c r="T25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U25" s="11">
+        <v>2</v>
+      </c>
+      <c r="V25" s="11">
+        <v>6</v>
+      </c>
+      <c r="W25" s="11">
+        <v>8</v>
+      </c>
+      <c r="X25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA25" s="11">
+        <v>6</v>
+      </c>
+      <c r="AB25" s="11">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AI25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK25" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO25" s="11">
+        <v>35</v>
+      </c>
+      <c r="AP25" s="11">
+        <v>20</v>
+      </c>
+      <c r="AQ25" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF25" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG25" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:59" s="11" customFormat="1">
+      <c r="A26" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="11">
+        <v>6</v>
+      </c>
+      <c r="G26" s="11">
+        <v>825</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0</v>
+      </c>
+      <c r="I26" s="11">
+        <v>1</v>
+      </c>
+      <c r="J26" s="11">
+        <v>4</v>
+      </c>
+      <c r="K26" s="11">
+        <v>6</v>
+      </c>
+      <c r="L26" s="11">
+        <v>4</v>
+      </c>
+      <c r="M26" s="11">
+        <v>1</v>
+      </c>
+      <c r="N26" s="11">
+        <v>2000</v>
+      </c>
+      <c r="O26" s="11">
+        <v>0</v>
+      </c>
+      <c r="P26" s="11">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>1</v>
+      </c>
+      <c r="R26" s="11">
+        <v>0</v>
+      </c>
+      <c r="S26" s="11">
+        <v>0</v>
+      </c>
+      <c r="T26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U26" s="11">
+        <v>4</v>
+      </c>
+      <c r="V26" s="11">
+        <v>7</v>
+      </c>
+      <c r="W26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="X26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA26" s="11">
+        <v>9</v>
+      </c>
+      <c r="AB26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="11">
+        <v>840</v>
+      </c>
+      <c r="AI26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK26" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO26" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP26" s="11">
+        <v>50</v>
+      </c>
+      <c r="AQ26" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF26" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG26" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:59" s="11" customFormat="1">
+      <c r="A28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="11">
+        <v>14</v>
+      </c>
+      <c r="G28" s="11">
+        <v>864</v>
+      </c>
+      <c r="H28" s="11">
+        <v>1</v>
+      </c>
+      <c r="I28" s="11">
+        <v>6</v>
+      </c>
+      <c r="J28" s="11">
+        <v>2</v>
+      </c>
+      <c r="K28" s="11">
+        <v>8</v>
+      </c>
+      <c r="L28" s="11">
+        <v>5</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0</v>
+      </c>
+      <c r="N28" s="11">
+        <v>1990</v>
+      </c>
+      <c r="O28" s="11">
+        <v>3</v>
+      </c>
+      <c r="P28" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>2</v>
+      </c>
+      <c r="R28" s="11">
+        <v>0</v>
+      </c>
+      <c r="S28" s="11">
+        <v>0</v>
+      </c>
+      <c r="T28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U28" s="11">
+        <v>3</v>
+      </c>
+      <c r="V28" s="11">
+        <v>0</v>
+      </c>
+      <c r="W28" s="11">
+        <v>1</v>
+      </c>
+      <c r="X28" s="11">
+        <v>3</v>
+      </c>
+      <c r="Y28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA28" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB28" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG28" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="11">
+        <v>800</v>
+      </c>
+      <c r="AI28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK28" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL28" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO28" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP28" s="11">
+        <v>75</v>
+      </c>
+      <c r="AQ28" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG28" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:59" s="11" customFormat="1">
+      <c r="A29" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="11">
+        <v>8</v>
+      </c>
+      <c r="G29" s="11">
+        <v>114</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1</v>
+      </c>
+      <c r="I29" s="11">
+        <v>7</v>
+      </c>
+      <c r="J29" s="11">
+        <v>7</v>
+      </c>
+      <c r="K29" s="11">
+        <v>4</v>
+      </c>
+      <c r="L29" s="11">
+        <v>5</v>
+      </c>
+      <c r="M29" s="11">
+        <v>1</v>
+      </c>
+      <c r="N29" s="11">
+        <v>2002</v>
+      </c>
+      <c r="O29" s="11">
+        <v>0</v>
+      </c>
+      <c r="P29" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>3</v>
+      </c>
+      <c r="R29" s="11">
+        <v>0</v>
+      </c>
+      <c r="S29" s="11">
+        <v>0</v>
+      </c>
+      <c r="T29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U29" s="11">
+        <v>5</v>
+      </c>
+      <c r="V29" s="11">
+        <v>0</v>
+      </c>
+      <c r="W29" s="11">
+        <v>0</v>
+      </c>
+      <c r="X29" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="11">
+        <v>1400</v>
+      </c>
+      <c r="AI29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK29" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO29" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP29" s="11">
+        <v>51</v>
+      </c>
+      <c r="AQ29" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG29" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59" s="11" customFormat="1">
+      <c r="A30" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="11">
+        <v>47</v>
+      </c>
+      <c r="G30" s="11">
+        <v>883</v>
+      </c>
+      <c r="H30" s="11">
+        <v>1</v>
+      </c>
+      <c r="I30" s="11">
+        <v>6</v>
+      </c>
+      <c r="J30" s="11">
+        <v>6</v>
+      </c>
+      <c r="K30" s="11">
+        <v>4</v>
+      </c>
+      <c r="L30" s="11">
+        <v>7</v>
+      </c>
+      <c r="M30" s="11">
+        <v>1</v>
+      </c>
+      <c r="N30" s="11">
+        <v>1995</v>
+      </c>
+      <c r="O30" s="11">
+        <v>0</v>
+      </c>
+      <c r="P30" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>2</v>
+      </c>
+      <c r="R30" s="11">
+        <v>0</v>
+      </c>
+      <c r="S30" s="11">
+        <v>2</v>
+      </c>
+      <c r="T30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U30" s="11">
+        <v>4</v>
+      </c>
+      <c r="V30" s="11">
+        <v>0</v>
+      </c>
+      <c r="W30" s="11">
+        <v>1</v>
+      </c>
+      <c r="X30" s="11">
+        <v>4</v>
+      </c>
+      <c r="Y30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA30" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB30" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC30" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="11">
+        <v>600</v>
+      </c>
+      <c r="AI30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK30" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL30" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO30" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP30" s="11">
+        <v>40</v>
+      </c>
+      <c r="AQ30" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG30" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59" s="11" customFormat="1">
+      <c r="A31" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="11">
+        <v>0</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="11">
+        <v>14</v>
+      </c>
+      <c r="G31" s="11">
+        <v>882</v>
+      </c>
+      <c r="H31" s="11">
+        <v>2</v>
+      </c>
+      <c r="I31" s="11">
+        <v>11</v>
+      </c>
+      <c r="J31" s="11">
+        <v>4</v>
+      </c>
+      <c r="K31" s="11">
+        <v>4</v>
+      </c>
+      <c r="L31" s="11">
+        <v>3</v>
+      </c>
+      <c r="M31" s="11">
+        <v>1</v>
+      </c>
+      <c r="N31" s="11">
+        <v>1985</v>
+      </c>
+      <c r="O31" s="11">
+        <v>2</v>
+      </c>
+      <c r="P31" s="11">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>1</v>
+      </c>
+      <c r="R31" s="11">
+        <v>0</v>
+      </c>
+      <c r="S31" s="11">
+        <v>0</v>
+      </c>
+      <c r="T31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U31" s="11">
+        <v>3</v>
+      </c>
+      <c r="V31" s="11">
+        <v>0</v>
+      </c>
+      <c r="W31" s="11">
+        <v>1</v>
+      </c>
+      <c r="X31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA31" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB31" s="11">
+        <v>6</v>
+      </c>
+      <c r="AC31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="11">
+        <v>2000</v>
+      </c>
+      <c r="AI31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK31" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL31" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO31" s="11">
+        <v>38</v>
+      </c>
+      <c r="AP31" s="11">
+        <v>38</v>
+      </c>
+      <c r="AQ31" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF31" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG31" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:59" s="11" customFormat="1">
+      <c r="A32" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="11">
+        <v>0</v>
+      </c>
+      <c r="C32" s="11">
+        <v>0</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="11">
+        <v>37</v>
+      </c>
+      <c r="G32" s="11">
+        <v>889</v>
+      </c>
+      <c r="H32" s="11">
+        <v>2</v>
+      </c>
+      <c r="I32" s="11">
+        <v>6</v>
+      </c>
+      <c r="J32" s="11">
+        <v>4</v>
+      </c>
+      <c r="K32" s="11">
+        <v>3</v>
+      </c>
+      <c r="L32" s="11">
+        <v>2</v>
+      </c>
+      <c r="M32" s="11">
+        <v>1</v>
+      </c>
+      <c r="N32" s="11">
+        <v>1991</v>
+      </c>
+      <c r="O32" s="11">
+        <v>3</v>
+      </c>
+      <c r="P32" s="11">
+        <v>40</v>
+      </c>
+      <c r="Q32" s="11">
+        <v>1</v>
+      </c>
+      <c r="R32" s="11">
+        <v>0</v>
+      </c>
+      <c r="S32" s="11">
+        <v>2</v>
+      </c>
+      <c r="T32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U32" s="11">
+        <v>2</v>
+      </c>
+      <c r="V32" s="11">
+        <v>1</v>
+      </c>
+      <c r="W32" s="11">
+        <v>0</v>
+      </c>
+      <c r="X32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA32" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB32" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC32" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG32" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="11">
+        <v>1600</v>
+      </c>
+      <c r="AI32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK32" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL32" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO32" s="11">
+        <v>38</v>
+      </c>
+      <c r="AP32" s="11">
+        <v>30</v>
+      </c>
+      <c r="AQ32" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF32" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG32" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:59" s="11" customFormat="1">
+      <c r="A33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="11">
+        <v>24</v>
+      </c>
+      <c r="G33" s="11">
+        <v>885</v>
+      </c>
+      <c r="H33" s="11">
+        <v>3</v>
+      </c>
+      <c r="I33" s="11">
+        <v>15</v>
+      </c>
+      <c r="J33" s="11">
+        <v>7</v>
+      </c>
+      <c r="K33" s="11">
+        <v>4</v>
+      </c>
+      <c r="L33" s="11">
+        <v>1</v>
+      </c>
+      <c r="M33" s="11">
+        <v>1</v>
+      </c>
+      <c r="N33" s="11">
+        <v>1997</v>
+      </c>
+      <c r="O33" s="11">
+        <v>4</v>
+      </c>
+      <c r="P33" s="11">
+        <v>30</v>
+      </c>
+      <c r="Q33" s="11">
+        <v>1</v>
+      </c>
+      <c r="R33" s="11">
+        <v>0</v>
+      </c>
+      <c r="S33" s="11">
+        <v>0</v>
+      </c>
+      <c r="T33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U33" s="11">
+        <v>1</v>
+      </c>
+      <c r="V33" s="11">
+        <v>3</v>
+      </c>
+      <c r="W33" s="11">
+        <v>4</v>
+      </c>
+      <c r="X33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA33" s="11">
+        <v>4</v>
+      </c>
+      <c r="AB33" s="11">
+        <v>6</v>
+      </c>
+      <c r="AC33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="11">
+        <v>1400</v>
+      </c>
+      <c r="AI33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK33" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO33" s="11">
+        <v>35</v>
+      </c>
+      <c r="AP33" s="11">
+        <v>10</v>
+      </c>
+      <c r="AQ33" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF33" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG33" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59" s="11" customFormat="1">
+      <c r="A34" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="11">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0</v>
+      </c>
+      <c r="D34" s="11">
+        <v>0</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="11">
+        <v>10</v>
+      </c>
+      <c r="G34" s="11">
+        <v>291</v>
+      </c>
+      <c r="H34" s="11">
+        <v>5</v>
+      </c>
+      <c r="I34" s="11">
+        <v>25</v>
+      </c>
+      <c r="J34" s="11">
+        <v>6</v>
+      </c>
+      <c r="K34" s="11">
+        <v>6</v>
+      </c>
+      <c r="L34" s="11">
+        <v>5</v>
+      </c>
+      <c r="M34" s="11">
+        <v>1</v>
+      </c>
+      <c r="N34" s="11">
+        <v>1999</v>
+      </c>
+      <c r="O34" s="11">
+        <v>4</v>
+      </c>
+      <c r="P34" s="11">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="11">
+        <v>1</v>
+      </c>
+      <c r="R34" s="11">
+        <v>0</v>
+      </c>
+      <c r="S34" s="11">
+        <v>0</v>
+      </c>
+      <c r="T34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U34" s="11">
+        <v>3</v>
+      </c>
+      <c r="V34" s="11">
+        <v>5</v>
+      </c>
+      <c r="W34" s="11">
+        <v>7</v>
+      </c>
+      <c r="X34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA34" s="11">
+        <v>6</v>
+      </c>
+      <c r="AB34" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="11">
+        <v>4000</v>
+      </c>
+      <c r="AI34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK34" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="11">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO34" s="11">
+        <v>35</v>
+      </c>
+      <c r="AP34" s="11">
+        <v>50</v>
+      </c>
+      <c r="AQ34" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF34" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG34" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:59" s="11" customFormat="1">
+      <c r="A35" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="11">
+        <v>0</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="11">
+        <v>0</v>
+      </c>
+      <c r="G35" s="11">
+        <v>823</v>
+      </c>
+      <c r="H35" s="11">
+        <v>4</v>
+      </c>
+      <c r="I35" s="11">
+        <v>18</v>
+      </c>
+      <c r="J35" s="11">
+        <v>5</v>
+      </c>
+      <c r="K35" s="11">
+        <v>3</v>
+      </c>
+      <c r="L35" s="11">
+        <v>4</v>
+      </c>
+      <c r="M35" s="11">
+        <v>1</v>
+      </c>
+      <c r="N35" s="11">
+        <v>1999</v>
+      </c>
+      <c r="O35" s="11">
+        <v>4</v>
+      </c>
+      <c r="P35" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="11">
+        <v>2</v>
+      </c>
+      <c r="R35" s="11">
+        <v>0</v>
+      </c>
+      <c r="S35" s="11">
+        <v>0</v>
+      </c>
+      <c r="T35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="U35" s="11">
+        <v>3</v>
+      </c>
+      <c r="V35" s="11">
+        <v>1</v>
+      </c>
+      <c r="W35" s="11">
+        <v>3</v>
+      </c>
+      <c r="X35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Y35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="Z35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AA35" s="11">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="11">
+        <v>8</v>
+      </c>
+      <c r="AC35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AG35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="11">
+        <v>800</v>
+      </c>
+      <c r="AI35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AJ35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AK35" s="11">
+        <v>90</v>
+      </c>
+      <c r="AL35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="11">
+        <v>5</v>
+      </c>
+      <c r="AN35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AO35" s="11">
+        <v>40</v>
+      </c>
+      <c r="AP35" s="11">
+        <v>60</v>
+      </c>
+      <c r="AQ35" s="11">
+        <v>10</v>
+      </c>
+      <c r="AR35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AS35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AT35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AU35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AV35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AW35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AX35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AY35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="AZ35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BA35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BB35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BC35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BD35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BE35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BF35" s="11">
+        <v>-1</v>
+      </c>
+      <c r="BG35" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Start working on Person, and finish Film
</commit_message>
<xml_diff>
--- a/Descriptive Data/pdata/FilmCompare.xlsx
+++ b/Descriptive Data/pdata/FilmCompare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>樂翻天新聞</t>
   </si>
@@ -75,211 +75,214 @@
     <t xml:space="preserve">與生活密切相關的醫學知識是每個國民都必須嘗試接觸的。                    </t>
   </si>
   <si>
+    <t>母親三十歲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本片洋溢人文主義的風彩，對於守寡婦女難耐的性慾寄予體諒之情。            </t>
+  </si>
+  <si>
+    <t>天涯歌女</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一代歌后周璇的故事。                                                    </t>
+  </si>
+  <si>
+    <t>雷瑪根鐵橋</t>
+  </si>
+  <si>
+    <t>我的美麗與哀愁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">以懸疑的情節，突破從校園到社會的重重禁忌，充分討論了青少年的蒙味感覺。  </t>
+  </si>
+  <si>
+    <t>影子軍團</t>
+  </si>
+  <si>
+    <t>坦克大決戰</t>
+  </si>
+  <si>
+    <t>二次世界大戰，德軍節節敗退之際，集中精銳的裝甲部隊與同盟國進行最後決戰。</t>
+  </si>
+  <si>
+    <t>轟炸超人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">代表正義與邪惡的超人們，將以手中的炸彈做勝負對決。                      </t>
+  </si>
+  <si>
+    <t>荒山孤墳</t>
+  </si>
+  <si>
+    <t>科學新疆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">科學知識日新月異，吸引著求知慾望強盛的人鑽研其中。                      </t>
+  </si>
+  <si>
+    <t>天堂旅行團</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">由靈異人士帶領，經由特殊儀式，讓靈魂出竅前往天堂參觀。                  </t>
+  </si>
+  <si>
+    <t>９９衝鋒飛車賽</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">講求速度與靈動的機車比賽是少年追風少年的最愛！                          </t>
+  </si>
+  <si>
+    <t>蜜桃成熟時</t>
+  </si>
+  <si>
+    <t xml:space="preserve">且看女主角如何經過歷練而成熟……                                        </t>
+  </si>
+  <si>
+    <t>Ｋ－１９</t>
+  </si>
+  <si>
+    <t>movi-a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蘇聯潛艇發生核能外洩意外，要如何挽救呢？                                </t>
+  </si>
+  <si>
+    <t>遠離家園</t>
+  </si>
+  <si>
+    <t>小甜甜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小甜甜從小生長在孤兒院，她既美麗又大方，是一個人見人愛的女子。          </t>
+  </si>
+  <si>
+    <t>大家來守法</t>
+  </si>
+  <si>
+    <t xml:space="preserve">各種生活中常遇到的法律問題。                                            </t>
+  </si>
+  <si>
+    <t>超級比一比　　　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">集合各種社會團體，在各項運動設施中拼一拼，看看誰奪得冠軍！              </t>
+  </si>
+  <si>
+    <t>龍舟大會</t>
+  </si>
+  <si>
+    <t>spe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龍舟中國節日的特有運動，講求團隊的默契。                                </t>
+  </si>
+  <si>
+    <t>片名</t>
+  </si>
+  <si>
+    <t>圖片檔</t>
+  </si>
+  <si>
+    <t>圖片ID</t>
+  </si>
+  <si>
+    <t>音效檔</t>
+  </si>
+  <si>
+    <t>大類別ID</t>
+  </si>
+  <si>
+    <t>子類型ID</t>
+  </si>
+  <si>
+    <t>評價</t>
+  </si>
+  <si>
+    <t>票房</t>
+  </si>
+  <si>
+    <t>卡士</t>
+  </si>
+  <si>
+    <t>普通級</t>
+  </si>
+  <si>
+    <t>年份</t>
+  </si>
+  <si>
+    <t>地區</t>
+  </si>
+  <si>
+    <t>集數</t>
+  </si>
+  <si>
+    <t>每集長度</t>
+  </si>
+  <si>
+    <t>?額外開機數</t>
+  </si>
+  <si>
+    <t>時代</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>製作等級</t>
+  </si>
+  <si>
+    <t>元素1ID</t>
+  </si>
+  <si>
+    <t>元素2ID</t>
+  </si>
+  <si>
+    <t>元素3ID</t>
+  </si>
+  <si>
+    <t>元素4ID</t>
+  </si>
+  <si>
+    <t>元素5ID</t>
+  </si>
+  <si>
+    <t>元素1比重</t>
+  </si>
+  <si>
+    <t>元素2比重</t>
+  </si>
+  <si>
+    <t>元素3比重</t>
+  </si>
+  <si>
+    <t>元素4比重</t>
+  </si>
+  <si>
+    <t>元素5比重</t>
+  </si>
+  <si>
     <t>售價</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>年份</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可播放次數</t>
+  </si>
+  <si>
+    <t>新鮮度</t>
   </si>
   <si>
     <t>強度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>新鮮度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>評價</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>票房</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡士</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>說明</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>集數</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>製作等級</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地區</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通級</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>片名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>子類型ID</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每集長度</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圖片檔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>大類別ID</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圖片ID</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>音效檔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>時代</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>?額外開機數</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>母親三十歲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">本片洋溢人文主義的風彩，對於守寡婦女難耐的性慾寄予體諒之情。            </t>
-  </si>
-  <si>
-    <t>天涯歌女</t>
-  </si>
-  <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">一代歌后周璇的故事。                                                    </t>
-  </si>
-  <si>
-    <t>可播放次數</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷瑪根鐵橋</t>
-  </si>
-  <si>
-    <t>?人氣</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>我的美麗與哀愁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">以懸疑的情節，突破從校園到社會的重重禁忌，充分討論了青少年的蒙味感覺。  </t>
-  </si>
-  <si>
-    <t>影子軍團</t>
-  </si>
-  <si>
-    <t>坦克大決戰</t>
-  </si>
-  <si>
-    <t>二次世界大戰，德軍節節敗退之際，集中精銳的裝甲部隊與同盟國進行最後決戰。</t>
-  </si>
-  <si>
-    <t>轟炸超人</t>
-  </si>
-  <si>
-    <t xml:space="preserve">代表正義與邪惡的超人們，將以手中的炸彈做勝負對決。                      </t>
-  </si>
-  <si>
-    <t>荒山孤墳</t>
-  </si>
-  <si>
-    <t>科學新疆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">科學知識日新月異，吸引著求知慾望強盛的人鑽研其中。                      </t>
-  </si>
-  <si>
-    <t>天堂旅行團</t>
-  </si>
-  <si>
-    <t>happy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">由靈異人士帶領，經由特殊儀式，讓靈魂出竅前往天堂參觀。                  </t>
-  </si>
-  <si>
-    <t>９９衝鋒飛車賽</t>
-  </si>
-  <si>
-    <t>sport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">講求速度與靈動的機車比賽是少年追風少年的最愛！                          </t>
-  </si>
-  <si>
-    <t>蜜桃成熟時</t>
-  </si>
-  <si>
-    <t xml:space="preserve">且看女主角如何經過歷練而成熟……                                        </t>
-  </si>
-  <si>
-    <t>Ｋ－１９</t>
-  </si>
-  <si>
-    <t>movi-a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">蘇聯潛艇發生核能外洩意外，要如何挽救呢？                                </t>
-  </si>
-  <si>
-    <t>遠離家園</t>
-  </si>
-  <si>
-    <t>小甜甜</t>
-  </si>
-  <si>
-    <t xml:space="preserve">小甜甜從小生長在孤兒院，她既美麗又大方，是一個人見人愛的女子。          </t>
-  </si>
-  <si>
-    <t>大家來守法</t>
-  </si>
-  <si>
-    <t xml:space="preserve">各種生活中常遇到的法律問題。                                            </t>
-  </si>
-  <si>
-    <t>超級比一比　　　</t>
-  </si>
-  <si>
-    <t xml:space="preserve">集合各種社會團體，在各項運動設施中拼一拼，看看誰奪得冠軍！              </t>
-  </si>
-  <si>
-    <t>龍舟大會</t>
-  </si>
-  <si>
-    <t>spe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">龍舟中國節日的特有運動，講求團隊的默契。                                </t>
   </si>
 </sst>
 </file>
@@ -1247,13 +1250,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="2.5" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="7.5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.5" bestFit="1" customWidth="1"/>
@@ -1265,10 +1266,8 @@
     <col min="19" max="19" width="5.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="31" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="31" width="10.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3.125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="2.75" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="5.5" bestFit="1" customWidth="1"/>
@@ -1286,145 +1285,172 @@
   <sheetData>
     <row r="1" spans="1:59" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>48</v>
+        <v>74</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="AF1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AG1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AH1" s="8" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="AI1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AK1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AL1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="AN1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AO1" s="8" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="AP1" s="8" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="AQ1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AR1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AS1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AT1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AU1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AV1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AW1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AX1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AY1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="AZ1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BA1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BB1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BC1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BD1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BE1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BF1" s="8" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="BG1" s="8" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:59">
@@ -2861,7 +2887,7 @@
     </row>
     <row r="13" spans="1:59">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -3035,12 +3061,12 @@
         <v>-1</v>
       </c>
       <c r="BG13" s="9" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:59">
       <c r="A14" s="11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B14" s="11">
         <v>0</v>
@@ -3052,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F14" s="11">
         <v>17</v>
@@ -3219,7 +3245,7 @@
     </row>
     <row r="15" spans="1:59">
       <c r="A15" s="10" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B15" s="10">
         <v>0</v>
@@ -3231,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F15" s="10">
         <v>37</v>
@@ -3393,12 +3419,12 @@
         <v>-1</v>
       </c>
       <c r="BG15" s="10" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:59" s="11" customFormat="1">
       <c r="A19" s="11" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B19" s="11">
         <v>0</v>
@@ -3572,12 +3598,12 @@
         <v>-1</v>
       </c>
       <c r="BG19" s="11" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:59" s="11" customFormat="1">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
@@ -3756,7 +3782,7 @@
     </row>
     <row r="21" spans="1:59" s="11" customFormat="1">
       <c r="A21" s="11" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B21" s="11">
         <v>0</v>
@@ -3930,12 +3956,12 @@
         <v>-1</v>
       </c>
       <c r="BG21" s="11" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:59" s="11" customFormat="1">
       <c r="A22" s="11" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B22" s="11">
         <v>0</v>
@@ -4109,12 +4135,12 @@
         <v>-1</v>
       </c>
       <c r="BG22" s="11" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:59" s="11" customFormat="1">
       <c r="A23" s="11" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B23" s="11">
         <v>0</v>
@@ -4293,7 +4319,7 @@
     </row>
     <row r="24" spans="1:59" s="11" customFormat="1">
       <c r="A24" s="11" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B24" s="11">
         <v>0</v>
@@ -4467,12 +4493,12 @@
         <v>-1</v>
       </c>
       <c r="BG24" s="11" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:59" s="11" customFormat="1">
       <c r="A25" s="11" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B25" s="11">
         <v>0</v>
@@ -4484,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F25" s="11">
         <v>10</v>
@@ -4646,12 +4672,12 @@
         <v>-1</v>
       </c>
       <c r="BG25" s="11" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:59" s="11" customFormat="1">
       <c r="A26" s="11" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B26" s="11">
         <v>0</v>
@@ -4663,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="F26" s="11">
         <v>6</v>
@@ -4825,12 +4851,12 @@
         <v>-1</v>
       </c>
       <c r="BG26" s="11" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:59" s="11" customFormat="1">
       <c r="A28" s="11" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B28" s="11">
         <v>0</v>
@@ -4842,7 +4868,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F28" s="11">
         <v>14</v>
@@ -5004,12 +5030,12 @@
         <v>-1</v>
       </c>
       <c r="BG28" s="11" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:59" s="11" customFormat="1">
       <c r="A29" s="11" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B29" s="11">
         <v>0</v>
@@ -5021,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="F29" s="11">
         <v>8</v>
@@ -5183,12 +5209,12 @@
         <v>-1</v>
       </c>
       <c r="BG29" s="11" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:59" s="11" customFormat="1">
       <c r="A30" s="11" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B30" s="11">
         <v>0</v>
@@ -5367,7 +5393,7 @@
     </row>
     <row r="31" spans="1:59" s="11" customFormat="1">
       <c r="A31" s="11" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B31" s="11">
         <v>0</v>
@@ -5541,12 +5567,12 @@
         <v>-1</v>
       </c>
       <c r="BG31" s="11" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:59" s="11" customFormat="1">
       <c r="A32" s="11" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B32" s="11">
         <v>0</v>
@@ -5558,7 +5584,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F32" s="11">
         <v>37</v>
@@ -5720,12 +5746,12 @@
         <v>-1</v>
       </c>
       <c r="BG32" s="11" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:59" s="11" customFormat="1">
       <c r="A33" s="11" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="B33" s="11">
         <v>0</v>
@@ -5899,12 +5925,12 @@
         <v>-1</v>
       </c>
       <c r="BG33" s="11" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:59" s="11" customFormat="1">
       <c r="A34" s="11" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="B34" s="11">
         <v>0</v>
@@ -5916,7 +5942,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F34" s="11">
         <v>10</v>
@@ -6078,12 +6104,12 @@
         <v>-1</v>
       </c>
       <c r="BG34" s="11" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:59" s="11" customFormat="1">
       <c r="A35" s="11" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B35" s="11">
         <v>0</v>
@@ -6095,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="F35" s="11">
         <v>0</v>
@@ -6257,7 +6283,7 @@
         <v>-1</v>
       </c>
       <c r="BG35" s="11" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>